<commit_message>
Update Peer Allocation (Blank).xlsx
</commit_message>
<xml_diff>
--- a/Peer Allocation (Blank).xlsx
+++ b/Peer Allocation (Blank).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KumruHolroyd\Documents\GitHub\UndergroundEscape\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub Repos\UnderGroundEscape\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED61AD60-690E-4E36-97F8-49F7B3F362F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2A276D-E5A6-463A-9BDC-7800D0E081A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -331,12 +331,12 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -348,7 +348,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -360,7 +360,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -374,21 +374,25 @@
       </c>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <v>100</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
       <c r="E4" s="2">
         <v>0</v>
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -402,7 +406,7 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -410,7 +414,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>

</xml_diff>